<commit_message>
planilha de risco atualizada
</commit_message>
<xml_diff>
--- a/Documentação/Planejamentos/Planilha de Riscos.xlsx
+++ b/Documentação/Planejamentos/Planilha de Riscos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -93,13 +93,16 @@
   </si>
   <si>
     <t>Troca de conhecimento e o "apadrinhamento" por aqueles que possuem mais conhecimento, para desenvolver a area com algum déficit.</t>
+  </si>
+  <si>
+    <t>Legenda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,16 +119,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -206,11 +232,114 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,6 +356,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -242,6 +412,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352040</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>56999</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="2733675"/>
+          <a:ext cx="3076190" cy="1209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:I10"/>
+  <dimension ref="C2:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="W16" sqref="T13:W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,8 +738,8 @@
     <col min="9" max="9" width="133.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C4" s="4">
         <v>1</v>
       </c>
@@ -572,7 +785,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C5" s="5">
         <v>2</v>
       </c>
@@ -595,7 +808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C6" s="5">
         <v>3</v>
       </c>
@@ -618,7 +831,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C7" s="5">
         <v>4</v>
       </c>
@@ -641,7 +854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <v>5</v>
       </c>
@@ -664,7 +877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>6</v>
       </c>
@@ -687,7 +900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C10" s="5">
         <v>7</v>
       </c>
@@ -710,8 +923,57 @@
         <v>22</v>
       </c>
     </row>
+    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="S11" s="23"/>
+      <c r="T11" s="24"/>
+    </row>
+    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="S12" s="19"/>
+      <c r="T12" s="20"/>
+      <c r="V12" s="17"/>
+    </row>
+    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="S13" s="21"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+    </row>
+    <row r="14" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+    </row>
+    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T15" s="7"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="16"/>
+    </row>
+    <row r="16" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T16" s="7"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="18"/>
+    </row>
+    <row r="17" spans="21:23" x14ac:dyDescent="0.25">
+      <c r="U17" s="11"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="13"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="D14:E14"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>